<commit_message>
admitting to use of excel
</commit_message>
<xml_diff>
--- a/assets/slides/acct3210/S5/E1.xlsx
+++ b/assets/slides/acct3210/S5/E1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shamussiothrun/ArthurHowardMorris.github.io/assets/slides/acct3210/S5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF6618E-F2A2-AD46-B7D0-2622330C3A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952B0942-CDBE-BF4B-8BDE-C901E30F102B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25640" yWindow="600" windowWidth="43700" windowHeight="42500" activeTab="4" xr2:uid="{97940E38-EABE-B149-AEE2-E79B4BA3DFD5}"/>
+    <workbookView xWindow="25640" yWindow="600" windowWidth="43700" windowHeight="42500" activeTab="3" xr2:uid="{97940E38-EABE-B149-AEE2-E79B4BA3DFD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Answer Report 1" sheetId="2" r:id="rId1"/>
@@ -3478,7 +3478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CBBAE6-BD52-C044-B026-6B818481B8A9}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
@@ -3763,7 +3763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD0FA63-7B82-AE47-97E6-E7327266E637}">
   <dimension ref="A1:E401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>

</xml_diff>